<commit_message>
Remove GitHub push instructions from README
</commit_message>
<xml_diff>
--- a/MY_COLLECTION_PRICES.xlsx
+++ b/MY_COLLECTION_PRICES.xlsx
@@ -467,7 +467,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -499,7 +499,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -527,7 +527,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>